<commit_message>
Zeiterfassung_Jeckle_Lukas.xlsx: Neuen Zeitposten gebucht.
Zeit zur Erstellung der GitHub Repository Grundstruktur gebucht.
</commit_message>
<xml_diff>
--- a/1. Projektplanung/1.1 Zeiterfassung/Zeiterfassung_Jeckle_Lukas.xlsx
+++ b/1. Projektplanung/1.1 Zeiterfassung/Zeiterfassung_Jeckle_Lukas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\FR1PEPF000013A3\EXCELCNV\b2533efa-3124-4889-a846-8594f2284b12\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thude0-my.sharepoint.com/personal/jecklu01_hs-ulm_de/Documents/5. Semester/Software Projekt/RaytRazor/1. Projektplanung/1.1 Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{C9F7BCB0-AC8D-48EA-AB1C-78C940CB4F06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACF85473-D0D0-4AE3-B8F0-8C2BC57FAA96}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{C9F7BCB0-AC8D-48EA-AB1C-78C940CB4F06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10057AF9-D249-4967-89B4-5FFF5EF1B427}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{60F36677-6C43-442F-912E-D347C7303937}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{60F36677-6C43-442F-912E-D347C7303937}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeiterfassung" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Name:</t>
   </si>
@@ -87,13 +87,16 @@
   </si>
   <si>
     <t>Projekt Kickoff Meeting.</t>
+  </si>
+  <si>
+    <t>Grundstruktur des GitHub Repositorys aufgebaut.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -442,13 +445,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBB1BBFA-3617-4C66-8A60-3FE210797165}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" style="2" customWidth="1"/>
@@ -457,7 +460,7 @@
     <col min="5" max="256" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -465,7 +468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -473,7 +476,7 @@
         <v>6003331</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -481,7 +484,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -489,7 +492,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -503,7 +506,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>45574</v>
       </c>
@@ -517,7 +520,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>45578</v>
       </c>
@@ -531,7 +534,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>45579</v>
       </c>
@@ -543,6 +546,20 @@
       </c>
       <c r="D9" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>45579</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -554,9 +571,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -704,22 +724,42 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F563E5B-E833-4685-AA5F-417D9097CE12}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F73990B7-24D7-4B3D-A03A-D9C83C8BF00B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17D4C286-40F8-430F-9A60-A6D20F13F078}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17D4C286-40F8-430F-9A60-A6D20F13F078}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bcfc458b-b0e2-47b4-8909-d39697dfebcc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F73990B7-24D7-4B3D-A03A-D9C83C8BF00B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F563E5B-E833-4685-AA5F-417D9097CE12}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>